<commit_message>
fix: add dataset for sentence NOSORTING
</commit_message>
<xml_diff>
--- a/detectors/sorting/dataset/dataset.xlsx
+++ b/detectors/sorting/dataset/dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Punya Orang\OKA\Kuli-ah\skripsi\new\evaluators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codes\nl2sql\detectors\sorting\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50600AD6-0926-4A7E-96FE-F62D60E415D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C37FD87-59FB-4992-BF29-6F3C90048A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="11625" xr2:uid="{3D9DA0B6-826C-439E-9C93-125696AA4C24}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3D9DA0B6-826C-439E-9C93-125696AA4C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="337">
   <si>
     <t>ASC</t>
   </si>
@@ -1012,6 +1012,39 @@
   </si>
   <si>
     <t>urutkan akun berdasarkan nama secara alfabetis dari Z ke A</t>
+  </si>
+  <si>
+    <t>Tampilkan semua data mahasiswa yang berasal dari jurusan Teknik Informatika.</t>
+  </si>
+  <si>
+    <t>Cari dosen yang memiliki NIP tertentu.</t>
+  </si>
+  <si>
+    <t>Tampilkan nama dan kode semua mata kuliah yang memiliki 3 SKS.</t>
+  </si>
+  <si>
+    <t>Ambil semua data kelas yang diajarkan pada semester ganjil tahun ajaran 2023/2024.</t>
+  </si>
+  <si>
+    <t>Tampilkan semua mahasiswa yang mengambil mata kuliah dengan nama "Struktur Data".</t>
+  </si>
+  <si>
+    <t>Cari mahasiswa yang lahir sebelum tahun 2000.</t>
+  </si>
+  <si>
+    <t>Tampilkan semua nilai huruf mahasiswa pada kelas tertentu.</t>
+  </si>
+  <si>
+    <t>Ambil data dosen yang mengajar lebih dari satu kelas.</t>
+  </si>
+  <si>
+    <t>Cari mahasiswa yang belum memiliki entri nilai.</t>
+  </si>
+  <si>
+    <t>Tampilkan mata kuliah yang tidak diambil oleh mahasiswa dengan NIM tertentu.</t>
+  </si>
+  <si>
+    <t>NOSORTING</t>
   </si>
 </sst>
 </file>
@@ -1414,20 +1447,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC51C9D5-2E9E-42BB-8962-2BFD719F9241}">
   <dimension ref="A1:E325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B246" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C256" sqref="C256"/>
+    <sheetView tabSelected="1" topLeftCell="A273" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A282" sqref="A282:A291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="75.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1444,7 +1477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1491,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1505,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1519,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1533,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1550,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1564,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1578,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1592,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1609,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1623,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1604,7 +1637,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1618,7 +1651,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1665,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1646,7 +1679,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1663,7 +1696,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +1710,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1691,7 +1724,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1708,7 +1741,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1725,7 +1758,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +1772,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1789,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1806,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1823,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1840,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1824,7 +1857,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1841,7 +1874,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1891,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1908,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1892,7 +1925,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +1942,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1926,7 +1959,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +1976,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1960,7 +1993,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1977,7 +2010,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +2027,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2011,7 +2044,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2028,7 +2061,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2045,7 +2078,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -2062,7 +2095,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -2079,7 +2112,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2096,7 +2129,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2113,7 +2146,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2163,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +2180,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2197,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2181,7 +2214,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2231,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2248,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2232,7 +2265,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2282,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -2266,7 +2299,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -2283,7 +2316,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2333,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -2317,7 +2350,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -2334,7 +2367,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -2351,7 +2384,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -2368,7 +2401,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -2385,7 +2418,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -2402,7 +2435,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -2419,7 +2452,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2436,7 +2469,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2453,7 +2486,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2503,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2487,7 +2520,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -2504,7 +2537,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2551,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2535,7 +2568,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2552,7 +2585,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2602,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2619,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -2603,7 +2636,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -2620,7 +2653,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -2637,7 +2670,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -2651,7 +2684,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -2668,7 +2701,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -2682,7 +2715,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -2699,7 +2732,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -2716,7 +2749,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -2733,7 +2766,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -2750,7 +2783,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -2767,7 +2800,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -2784,7 +2817,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2801,7 +2834,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -2818,7 +2851,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -2835,7 +2868,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -2852,7 +2885,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +2902,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -2886,7 +2919,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -2903,7 +2936,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -2920,7 +2953,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -2937,7 +2970,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -2954,7 +2987,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -2971,7 +3004,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -2988,7 +3021,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -3005,7 +3038,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -3022,7 +3055,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -3039,7 +3072,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -3056,7 +3089,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -3073,7 +3106,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3123,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -3107,7 +3140,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -3124,7 +3157,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -3141,7 +3174,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3191,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -3175,7 +3208,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3225,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -3209,7 +3242,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -3226,7 +3259,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -3243,7 +3276,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -3260,7 +3293,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -3277,7 +3310,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -3294,7 +3327,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -3311,7 +3344,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -3328,7 +3361,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -3345,7 +3378,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -3362,7 +3395,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -3379,7 +3412,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -3396,7 +3429,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -3413,7 +3446,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -3430,7 +3463,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -3447,7 +3480,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -3464,7 +3497,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -3481,7 +3514,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -3498,7 +3531,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3548,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -3532,7 +3565,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -3549,7 +3582,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -3566,7 +3599,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -3583,7 +3616,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3630,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>1</v>
       </c>
@@ -3614,7 +3647,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -3631,7 +3664,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -3648,7 +3681,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -3665,7 +3698,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>1</v>
       </c>
@@ -3682,7 +3715,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>1</v>
       </c>
@@ -3699,7 +3732,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -3716,7 +3749,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -3733,7 +3766,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>1</v>
       </c>
@@ -3750,7 +3783,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -3764,7 +3797,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -3781,7 +3814,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -3798,7 +3831,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -3815,7 +3848,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -3832,7 +3865,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -3849,7 +3882,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -3866,7 +3899,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -3883,7 +3916,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -3900,7 +3933,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3950,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -3934,7 +3967,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>1</v>
       </c>
@@ -3951,7 +3984,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -3968,7 +4001,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -3985,7 +4018,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -4002,7 +4035,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -4019,7 +4052,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -4036,7 +4069,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>1</v>
       </c>
@@ -4053,7 +4086,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>1</v>
       </c>
@@ -4070,7 +4103,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>1</v>
       </c>
@@ -4087,7 +4120,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>1</v>
       </c>
@@ -4104,7 +4137,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -4121,7 +4154,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -4138,7 +4171,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -4155,7 +4188,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -4172,7 +4205,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -4189,7 +4222,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -4206,7 +4239,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -4223,7 +4256,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4273,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -4254,7 +4287,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -4271,7 +4304,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>1</v>
       </c>
@@ -4288,7 +4321,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>1</v>
       </c>
@@ -4305,7 +4338,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>1</v>
       </c>
@@ -4322,7 +4355,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>1</v>
       </c>
@@ -4339,7 +4372,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>1</v>
       </c>
@@ -4356,7 +4389,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>1</v>
       </c>
@@ -4373,7 +4406,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>1</v>
       </c>
@@ -4390,7 +4423,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>1</v>
       </c>
@@ -4407,7 +4440,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>1</v>
       </c>
@@ -4421,7 +4454,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>1</v>
       </c>
@@ -4438,7 +4471,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -4455,7 +4488,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -4472,7 +4505,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -4489,7 +4522,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -4506,7 +4539,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -4523,7 +4556,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -4540,7 +4573,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -4557,7 +4590,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -4574,7 +4607,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -4591,7 +4624,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -4608,7 +4641,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>1</v>
       </c>
@@ -4625,7 +4658,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>1</v>
       </c>
@@ -4642,7 +4675,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>1</v>
       </c>
@@ -4659,7 +4692,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>1</v>
       </c>
@@ -4676,7 +4709,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>1</v>
       </c>
@@ -4693,7 +4726,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>1</v>
       </c>
@@ -4710,7 +4743,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>1</v>
       </c>
@@ -4727,7 +4760,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>1</v>
       </c>
@@ -4744,7 +4777,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>1</v>
       </c>
@@ -4761,7 +4794,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>1</v>
       </c>
@@ -4778,7 +4811,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -4795,7 +4828,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -4812,7 +4845,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -4829,7 +4862,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -4846,7 +4879,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -4863,7 +4896,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -4880,7 +4913,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>0</v>
       </c>
@@ -4897,7 +4930,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -4914,7 +4947,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -4931,7 +4964,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -4948,7 +4981,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>1</v>
       </c>
@@ -4965,7 +4998,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>1</v>
       </c>
@@ -4982,7 +5015,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>1</v>
       </c>
@@ -4999,7 +5032,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>1</v>
       </c>
@@ -5016,7 +5049,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>1</v>
       </c>
@@ -5033,7 +5066,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>1</v>
       </c>
@@ -5050,7 +5083,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>1</v>
       </c>
@@ -5067,7 +5100,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>1</v>
       </c>
@@ -5084,7 +5117,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>1</v>
       </c>
@@ -5101,7 +5134,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>1</v>
       </c>
@@ -5118,7 +5151,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -5135,7 +5168,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -5152,7 +5185,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -5169,7 +5202,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -5186,7 +5219,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -5203,7 +5236,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -5220,7 +5253,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -5237,7 +5270,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -5254,7 +5287,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -5271,7 +5304,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -5288,7 +5321,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>1</v>
       </c>
@@ -5305,7 +5338,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>1</v>
       </c>
@@ -5322,7 +5355,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>1</v>
       </c>
@@ -5339,7 +5372,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>1</v>
       </c>
@@ -5356,7 +5389,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>1</v>
       </c>
@@ -5373,7 +5406,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>1</v>
       </c>
@@ -5390,7 +5423,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>1</v>
       </c>
@@ -5407,7 +5440,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>1</v>
       </c>
@@ -5424,7 +5457,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>1</v>
       </c>
@@ -5441,7 +5474,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>1</v>
       </c>
@@ -5458,7 +5491,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -5475,7 +5508,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -5492,7 +5525,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -5509,7 +5542,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -5526,7 +5559,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -5543,7 +5576,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -5560,7 +5593,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -5577,7 +5610,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -5594,7 +5627,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -5611,7 +5644,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -5628,7 +5661,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>1</v>
       </c>
@@ -5645,7 +5678,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -5662,7 +5695,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>1</v>
       </c>
@@ -5679,7 +5712,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>1</v>
       </c>
@@ -5696,7 +5729,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>1</v>
       </c>
@@ -5713,7 +5746,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>1</v>
       </c>
@@ -5730,7 +5763,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>1</v>
       </c>
@@ -5747,7 +5780,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -5764,7 +5797,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>1</v>
       </c>
@@ -5781,7 +5814,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>1</v>
       </c>
@@ -5798,7 +5831,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -5815,7 +5848,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>0</v>
       </c>
@@ -5832,7 +5865,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>0</v>
       </c>
@@ -5849,7 +5882,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>0</v>
       </c>
@@ -5866,7 +5899,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>0</v>
       </c>
@@ -5883,7 +5916,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -5900,7 +5933,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>0</v>
       </c>
@@ -5917,7 +5950,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>0</v>
       </c>
@@ -5934,7 +5967,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>0</v>
       </c>
@@ -5951,7 +5984,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>0</v>
       </c>
@@ -5968,7 +6001,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>1</v>
       </c>
@@ -5985,7 +6018,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>1</v>
       </c>
@@ -6002,7 +6035,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>1</v>
       </c>
@@ -6019,7 +6052,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>1</v>
       </c>
@@ -6036,7 +6069,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>1</v>
       </c>
@@ -6053,7 +6086,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>1</v>
       </c>
@@ -6070,7 +6103,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>1</v>
       </c>
@@ -6087,7 +6120,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>1</v>
       </c>
@@ -6104,7 +6137,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>1</v>
       </c>
@@ -6121,7 +6154,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>1</v>
       </c>
@@ -6138,124 +6171,216 @@
         <v>310</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B286"/>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B287"/>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B288"/>
-    </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B289"/>
-    </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B290"/>
-    </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B291"/>
-    </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>336</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C282" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>336</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C283" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>336</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C284" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>336</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C285" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>336</v>
+      </c>
+      <c r="B286" t="s">
+        <v>330</v>
+      </c>
+      <c r="C286" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>336</v>
+      </c>
+      <c r="B287" t="s">
+        <v>331</v>
+      </c>
+      <c r="C287" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>336</v>
+      </c>
+      <c r="B288" t="s">
+        <v>332</v>
+      </c>
+      <c r="C288" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>336</v>
+      </c>
+      <c r="B289" t="s">
+        <v>333</v>
+      </c>
+      <c r="C289" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>336</v>
+      </c>
+      <c r="B290" t="s">
+        <v>334</v>
+      </c>
+      <c r="C290" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>336</v>
+      </c>
+      <c r="B291" t="s">
+        <v>335</v>
+      </c>
+      <c r="C291" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B292"/>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B293"/>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B294"/>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B295"/>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B296"/>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B297"/>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B298"/>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B299"/>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B300"/>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B301"/>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B302"/>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B303"/>
     </row>
-    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B304"/>
     </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B305"/>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B306"/>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B307"/>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B308"/>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B309"/>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B310"/>
     </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B311"/>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B312"/>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B313"/>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B314"/>
     </row>
-    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B315"/>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B316"/>
     </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B317"/>
     </row>
-    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B318"/>
     </row>
-    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B319"/>
     </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B320"/>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B321"/>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B322"/>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B323"/>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B324"/>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B325"/>
     </row>
   </sheetData>

</xml_diff>